<commit_message>
Changed to new weight
</commit_message>
<xml_diff>
--- a/data/运行结果.xlsx
+++ b/data/运行结果.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wangyw15\Desktop\2023E\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8452B663-2954-4AAB-A933-400CC893D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26CEFC4-247E-420D-A500-CCD57DFB64D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2230" yWindow="1250" windowWidth="21300" windowHeight="12430" xr2:uid="{A5272FD2-90F1-414B-AE3A-6FE74AD8A7CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A5272FD2-90F1-414B-AE3A-6FE74AD8A7CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.48414000000000001</v>
+        <v>0.60753999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.43901000000000001</v>
+        <v>0.69030999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -480,7 +480,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.58611999999999997</v>
+        <v>0.59492</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -488,7 +488,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.52997000000000005</v>
+        <v>0.59145999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -496,7 +496,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.24043</v>
+        <v>0.48859000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.15503</v>
+        <v>0.40660000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>7.6082999999999998E-2</v>
+        <v>0.38080999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -520,7 +520,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.10027</v>
+        <v>0.36770000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -528,7 +528,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.10161000000000001</v>
+        <v>0.40527000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -536,7 +536,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5.0744999999999998E-2</v>
+        <v>0.18786</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -544,7 +544,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5.9369999999999999E-2</v>
+        <v>0.34936</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -552,7 +552,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>4.9783000000000001E-2</v>
+        <v>0.21362999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>